<commit_message>
Avances de una semana
</commit_message>
<xml_diff>
--- a/articulo_dfa/Hurst/Source_vale2.xlsx
+++ b/articulo_dfa/Hurst/Source_vale2.xlsx
@@ -604,10 +604,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB91"/>
+  <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1500" activePane="bottomLeft"/>
+      <selection activeCell="X80" sqref="X80"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7546,8 +7548,12 @@
       <c r="F82" s="10">
         <v>368</v>
       </c>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
+      <c r="G82">
+        <v>1.4843218269321701</v>
+      </c>
+      <c r="H82">
+        <v>1.5381694804222401</v>
+      </c>
       <c r="I82" s="12">
         <v>1.4284443929999999</v>
       </c>
@@ -7628,8 +7634,12 @@
       <c r="F83" s="10">
         <v>370</v>
       </c>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
+      <c r="G83">
+        <v>1.5044411195773499</v>
+      </c>
+      <c r="H83">
+        <v>1.5375297392573599</v>
+      </c>
       <c r="I83" s="12">
         <v>1.411779983</v>
       </c>
@@ -7710,8 +7720,12 @@
       <c r="F84" s="10">
         <v>371</v>
       </c>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
+      <c r="G84">
+        <v>1.57456325667648</v>
+      </c>
+      <c r="H84">
+        <v>1.5958824390773201</v>
+      </c>
       <c r="I84" s="12">
         <v>1.4253587400000001</v>
       </c>
@@ -7792,8 +7806,12 @@
       <c r="F85" s="10">
         <v>372</v>
       </c>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
+      <c r="G85">
+        <v>1.4540242931907701</v>
+      </c>
+      <c r="H85">
+        <v>1.6276491655557801</v>
+      </c>
       <c r="I85" s="12">
         <v>1.5444303450000001</v>
       </c>
@@ -7874,8 +7892,12 @@
       <c r="F86" s="10">
         <v>373</v>
       </c>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
+      <c r="G86">
+        <v>1.53339086262489</v>
+      </c>
+      <c r="H86">
+        <v>1.5681570740578401</v>
+      </c>
       <c r="I86" s="12">
         <v>1.521924651</v>
       </c>
@@ -7956,8 +7978,12 @@
       <c r="F87" s="10">
         <v>374</v>
       </c>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
+      <c r="G87">
+        <v>1.46808631572044</v>
+      </c>
+      <c r="H87">
+        <v>1.5036772509418199</v>
+      </c>
       <c r="I87" s="12">
         <v>1.5057655109999999</v>
       </c>
@@ -8038,8 +8064,12 @@
       <c r="F88" s="10">
         <v>375</v>
       </c>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
+      <c r="G88">
+        <v>1.61672031117685</v>
+      </c>
+      <c r="H88">
+        <v>1.6002723116586099</v>
+      </c>
       <c r="I88" s="12">
         <v>1.5993774279999999</v>
       </c>
@@ -8120,8 +8150,12 @@
       <c r="F89" s="10">
         <v>376</v>
       </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
+      <c r="G89">
+        <v>1.55259740450018</v>
+      </c>
+      <c r="H89">
+        <v>1.5215908670937</v>
+      </c>
       <c r="I89" s="12">
         <v>1.4667739719999999</v>
       </c>
@@ -8202,8 +8236,12 @@
       <c r="F90" s="10">
         <v>377</v>
       </c>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
+      <c r="G90">
+        <v>1.5344934521746401</v>
+      </c>
+      <c r="H90">
+        <v>1.5437936588057299</v>
+      </c>
       <c r="I90" s="12">
         <v>1.5866407279999999</v>
       </c>
@@ -8284,8 +8322,12 @@
       <c r="F91" s="10">
         <v>378</v>
       </c>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
+      <c r="G91">
+        <v>1.47414226596537</v>
+      </c>
+      <c r="H91">
+        <v>1.5337525885385199</v>
+      </c>
       <c r="I91" s="12">
         <v>1.5398369460000001</v>
       </c>
@@ -8347,7 +8389,868 @@
         <v>0.66018030029999997</v>
       </c>
     </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>10</v>
+      </c>
+      <c r="B92" s="15">
+        <v>73</v>
+      </c>
+      <c r="C92" s="22">
+        <v>29</v>
+      </c>
+      <c r="D92" s="22">
+        <v>96</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+      <c r="F92" s="10">
+        <v>113</v>
+      </c>
+      <c r="G92">
+        <v>1.6251179340523001</v>
+      </c>
+      <c r="H92">
+        <v>1.6059984228511199</v>
+      </c>
+      <c r="I92">
+        <v>1.40420055191917</v>
+      </c>
+      <c r="J92">
+        <v>1.4870456491346999</v>
+      </c>
+      <c r="K92">
+        <v>1.4678133899538</v>
+      </c>
+      <c r="L92">
+        <v>1.4907849276101599</v>
+      </c>
+      <c r="M92">
+        <v>1.2876418810834001</v>
+      </c>
+      <c r="N92">
+        <v>1.38978979989828</v>
+      </c>
+      <c r="O92">
+        <v>1.34542571467574</v>
+      </c>
+      <c r="P92">
+        <v>1.4063860582793399</v>
+      </c>
+      <c r="Q92">
+        <v>1.3062531371684001</v>
+      </c>
+      <c r="R92">
+        <v>1.35313140320329</v>
+      </c>
+      <c r="S92">
+        <v>1.34468068038636</v>
+      </c>
+      <c r="T92">
+        <v>1.3714087507472299</v>
+      </c>
+      <c r="U92">
+        <v>1.3904272730651901</v>
+      </c>
+      <c r="V92">
+        <v>1.39287108969474</v>
+      </c>
+      <c r="W92">
+        <v>1.5079377506020499</v>
+      </c>
+      <c r="X92">
+        <v>1.35560631264559</v>
+      </c>
+      <c r="Y92">
+        <v>1.3616555467778699</v>
+      </c>
+      <c r="Z92">
+        <v>1.6352856853347799</v>
+      </c>
+      <c r="AA92">
+        <v>1.46910708922918</v>
+      </c>
+      <c r="AB92">
+        <v>0.886913148907163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
+        <v>10</v>
+      </c>
+      <c r="B93" s="15">
+        <v>73</v>
+      </c>
+      <c r="C93" s="22">
+        <v>29</v>
+      </c>
+      <c r="D93" s="22">
+        <v>96</v>
+      </c>
+      <c r="E93" s="1">
+        <v>2</v>
+      </c>
+      <c r="F93" s="10">
+        <v>117</v>
+      </c>
+      <c r="G93">
+        <v>1.5935513001602599</v>
+      </c>
+      <c r="H93">
+        <v>1.6094334753528099</v>
+      </c>
+      <c r="I93">
+        <v>1.6030574587739701</v>
+      </c>
+      <c r="J93">
+        <v>1.63172749880989</v>
+      </c>
+      <c r="K93">
+        <v>1.5765074853544201</v>
+      </c>
+      <c r="L93">
+        <v>1.59181910905311</v>
+      </c>
+      <c r="M93">
+        <v>1.60794576396712</v>
+      </c>
+      <c r="N93">
+        <v>1.6316801143058699</v>
+      </c>
+      <c r="O93">
+        <v>1.57438769353093</v>
+      </c>
+      <c r="P93">
+        <v>1.5819586865898101</v>
+      </c>
+      <c r="Q93">
+        <v>1.60726232594227</v>
+      </c>
+      <c r="R93">
+        <v>1.62305678146342</v>
+      </c>
+      <c r="S93">
+        <v>1.5836342111063999</v>
+      </c>
+      <c r="T93">
+        <v>1.5920383508486899</v>
+      </c>
+      <c r="U93">
+        <v>1.5826461219149299</v>
+      </c>
+      <c r="V93">
+        <v>1.59811026388662</v>
+      </c>
+      <c r="W93">
+        <v>1.58521604859882</v>
+      </c>
+      <c r="X93">
+        <v>1.56203705963327</v>
+      </c>
+      <c r="Y93">
+        <v>1.57125044577557</v>
+      </c>
+      <c r="Z93">
+        <v>1.6002033616376701</v>
+      </c>
+      <c r="AA93">
+        <v>1.5283483889818099</v>
+      </c>
+      <c r="AB93">
+        <v>0.53320855712386594</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A94" s="9">
+        <v>10</v>
+      </c>
+      <c r="B94" s="15">
+        <v>73</v>
+      </c>
+      <c r="C94" s="22">
+        <v>29</v>
+      </c>
+      <c r="D94" s="22">
+        <v>96</v>
+      </c>
+      <c r="E94" s="1">
+        <v>3</v>
+      </c>
+      <c r="F94" s="10">
+        <v>118</v>
+      </c>
+      <c r="G94">
+        <v>1.8241122040336299</v>
+      </c>
+      <c r="H94">
+        <v>1.8345502449745901</v>
+      </c>
+      <c r="I94">
+        <v>1.7991950297239201</v>
+      </c>
+      <c r="J94">
+        <v>1.8342908794339501</v>
+      </c>
+      <c r="K94">
+        <v>1.7856901439311299</v>
+      </c>
+      <c r="L94">
+        <v>1.8015934721283899</v>
+      </c>
+      <c r="M94">
+        <v>1.8154755668331699</v>
+      </c>
+      <c r="N94">
+        <v>1.84062865320111</v>
+      </c>
+      <c r="O94">
+        <v>1.7700679878738199</v>
+      </c>
+      <c r="P94">
+        <v>1.77899348404372</v>
+      </c>
+      <c r="Q94">
+        <v>1.8131210454034199</v>
+      </c>
+      <c r="R94">
+        <v>1.83164316386468</v>
+      </c>
+      <c r="S94">
+        <v>1.78850314009975</v>
+      </c>
+      <c r="T94">
+        <v>1.7903377562479901</v>
+      </c>
+      <c r="U94">
+        <v>1.78929754203517</v>
+      </c>
+      <c r="V94">
+        <v>1.80199803648933</v>
+      </c>
+      <c r="W94">
+        <v>1.78915118348471</v>
+      </c>
+      <c r="X94">
+        <v>1.7545388607224399</v>
+      </c>
+      <c r="Y94">
+        <v>1.7750946195620301</v>
+      </c>
+      <c r="Z94">
+        <v>1.7701714141781699</v>
+      </c>
+      <c r="AA94">
+        <v>1.6779485373937799</v>
+      </c>
+      <c r="AB94">
+        <v>0.49056438361388799</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A95" s="9">
+        <v>10</v>
+      </c>
+      <c r="B95" s="15">
+        <v>73</v>
+      </c>
+      <c r="C95" s="22">
+        <v>29</v>
+      </c>
+      <c r="D95" s="22">
+        <v>96</v>
+      </c>
+      <c r="E95" s="1">
+        <v>4</v>
+      </c>
+      <c r="F95" s="10">
+        <v>131</v>
+      </c>
+      <c r="G95">
+        <v>1.76606856312885</v>
+      </c>
+      <c r="H95">
+        <v>1.74292679209502</v>
+      </c>
+      <c r="I95">
+        <v>1.6893425150357699</v>
+      </c>
+      <c r="J95">
+        <v>1.69818243433786</v>
+      </c>
+      <c r="K95">
+        <v>1.66752769294499</v>
+      </c>
+      <c r="L95">
+        <v>1.6618703983904799</v>
+      </c>
+      <c r="M95">
+        <v>1.67729338874125</v>
+      </c>
+      <c r="N95">
+        <v>1.70152990103558</v>
+      </c>
+      <c r="O95">
+        <v>1.61773792132616</v>
+      </c>
+      <c r="P95">
+        <v>1.6221356600837999</v>
+      </c>
+      <c r="Q95">
+        <v>1.6553417163829001</v>
+      </c>
+      <c r="R95">
+        <v>1.6740613761666101</v>
+      </c>
+      <c r="S95">
+        <v>1.6309543636049699</v>
+      </c>
+      <c r="T95">
+        <v>1.6350501813573</v>
+      </c>
+      <c r="U95">
+        <v>1.63499935310664</v>
+      </c>
+      <c r="V95">
+        <v>1.6542325059865099</v>
+      </c>
+      <c r="W95">
+        <v>1.6628347911082899</v>
+      </c>
+      <c r="X95">
+        <v>1.6015990820124999</v>
+      </c>
+      <c r="Y95">
+        <v>1.6179121657584801</v>
+      </c>
+      <c r="Z95">
+        <v>1.5907151197809499</v>
+      </c>
+      <c r="AA95">
+        <v>1.5252807883900299</v>
+      </c>
+      <c r="AB95">
+        <v>0.65947336213993402</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A96" s="9">
+        <v>10</v>
+      </c>
+      <c r="B96" s="15">
+        <v>73</v>
+      </c>
+      <c r="C96" s="22">
+        <v>29</v>
+      </c>
+      <c r="D96" s="22">
+        <v>96</v>
+      </c>
+      <c r="E96" s="1">
+        <v>5</v>
+      </c>
+      <c r="F96" s="10">
+        <v>422</v>
+      </c>
+      <c r="G96">
+        <v>1.2821538617008099</v>
+      </c>
+      <c r="H96">
+        <v>1.3104771155541599</v>
+      </c>
+      <c r="I96">
+        <v>1.14791025848763</v>
+      </c>
+      <c r="J96">
+        <v>1.16741859187383</v>
+      </c>
+      <c r="K96">
+        <v>1.1209004023109099</v>
+      </c>
+      <c r="L96">
+        <v>1.1956936227310699</v>
+      </c>
+      <c r="M96">
+        <v>1.0691461222627101</v>
+      </c>
+      <c r="N96">
+        <v>1.1551559910498399</v>
+      </c>
+      <c r="O96">
+        <v>1.10464898970504</v>
+      </c>
+      <c r="P96">
+        <v>1.1329005381707999</v>
+      </c>
+      <c r="Q96">
+        <v>0.999383455989452</v>
+      </c>
+      <c r="R96">
+        <v>1.11300220724016</v>
+      </c>
+      <c r="S96">
+        <v>1.13968275893839</v>
+      </c>
+      <c r="T96">
+        <v>1.4595777403400101</v>
+      </c>
+      <c r="U96">
+        <v>1.19622596310957</v>
+      </c>
+      <c r="V96">
+        <v>1.1859976815276101</v>
+      </c>
+      <c r="W96">
+        <v>1.10173437938486</v>
+      </c>
+      <c r="X96">
+        <v>1.1145946415777499</v>
+      </c>
+      <c r="Y96">
+        <v>1.0914142781129299</v>
+      </c>
+      <c r="Z96">
+        <v>1.3233110560317201</v>
+      </c>
+      <c r="AA96">
+        <v>1.26640260971258</v>
+      </c>
+      <c r="AB96">
+        <v>0.44270815753048298</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A97" s="9">
+        <v>10</v>
+      </c>
+      <c r="B97" s="15">
+        <v>73</v>
+      </c>
+      <c r="C97" s="22">
+        <v>29</v>
+      </c>
+      <c r="D97" s="22">
+        <v>96</v>
+      </c>
+      <c r="E97" s="1">
+        <v>6</v>
+      </c>
+      <c r="F97" s="10">
+        <v>606</v>
+      </c>
+      <c r="G97">
+        <v>1.5240341456075499</v>
+      </c>
+      <c r="H97">
+        <v>1.4571857678664</v>
+      </c>
+      <c r="I97">
+        <v>1.6587147425308899</v>
+      </c>
+      <c r="J97">
+        <v>1.42821148792254</v>
+      </c>
+      <c r="K97">
+        <v>1.3677163384689699</v>
+      </c>
+      <c r="L97">
+        <v>1.40129935698116</v>
+      </c>
+      <c r="M97">
+        <v>1.3944384863930801</v>
+      </c>
+      <c r="N97">
+        <v>1.35883835546396</v>
+      </c>
+      <c r="O97">
+        <v>1.3384219491016001</v>
+      </c>
+      <c r="P97">
+        <v>1.35837252008734</v>
+      </c>
+      <c r="Q97">
+        <v>1.3485409738868399</v>
+      </c>
+      <c r="R97">
+        <v>1.3223980545529901</v>
+      </c>
+      <c r="S97">
+        <v>1.3345791029796099</v>
+      </c>
+      <c r="T97">
+        <v>1.3465081852730201</v>
+      </c>
+      <c r="U97">
+        <v>1.31593657813844</v>
+      </c>
+      <c r="V97">
+        <v>1.29444856768883</v>
+      </c>
+      <c r="W97">
+        <v>1.3533467542339801</v>
+      </c>
+      <c r="X97">
+        <v>1.3258344140004901</v>
+      </c>
+      <c r="Y97">
+        <v>1.3282829601898201</v>
+      </c>
+      <c r="Z97">
+        <v>1.5942380975380801</v>
+      </c>
+      <c r="AA97">
+        <v>1.4159509517839</v>
+      </c>
+      <c r="AB97">
+        <v>0.55376139276247205</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
+        <v>10</v>
+      </c>
+      <c r="B98" s="15">
+        <v>73</v>
+      </c>
+      <c r="C98" s="22">
+        <v>29</v>
+      </c>
+      <c r="D98" s="22">
+        <v>96</v>
+      </c>
+      <c r="E98" s="1">
+        <v>7</v>
+      </c>
+      <c r="F98" s="10">
+        <v>607</v>
+      </c>
+      <c r="G98">
+        <v>1.4304081788984599</v>
+      </c>
+      <c r="H98">
+        <v>1.4723447023318801</v>
+      </c>
+      <c r="I98">
+        <v>1.79161723696458</v>
+      </c>
+      <c r="J98">
+        <v>1.3904980366538</v>
+      </c>
+      <c r="K98">
+        <v>1.34824180601461</v>
+      </c>
+      <c r="L98">
+        <v>1.3733514866494001</v>
+      </c>
+      <c r="M98">
+        <v>1.38754518976029</v>
+      </c>
+      <c r="N98">
+        <v>1.3521648211886499</v>
+      </c>
+      <c r="O98">
+        <v>1.2905711833454401</v>
+      </c>
+      <c r="P98">
+        <v>1.3356890901663101</v>
+      </c>
+      <c r="Q98">
+        <v>1.31505913832125</v>
+      </c>
+      <c r="R98">
+        <v>1.29167998104299</v>
+      </c>
+      <c r="S98">
+        <v>1.2965484250189701</v>
+      </c>
+      <c r="T98">
+        <v>1.38658504669788</v>
+      </c>
+      <c r="U98">
+        <v>1.2804477652997099</v>
+      </c>
+      <c r="V98">
+        <v>1.2683354268209199</v>
+      </c>
+      <c r="W98">
+        <v>1.35523313546669</v>
+      </c>
+      <c r="X98">
+        <v>1.2847415447287001</v>
+      </c>
+      <c r="Y98">
+        <v>1.28363113520674</v>
+      </c>
+      <c r="Z98">
+        <v>1.55519854022432</v>
+      </c>
+      <c r="AA98">
+        <v>1.4397620822457999</v>
+      </c>
+      <c r="AB98">
+        <v>0.56795348406665402</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A99" s="9">
+        <v>10</v>
+      </c>
+      <c r="B99" s="15">
+        <v>73</v>
+      </c>
+      <c r="C99" s="22">
+        <v>29</v>
+      </c>
+      <c r="D99" s="22">
+        <v>96</v>
+      </c>
+      <c r="E99" s="1">
+        <v>8</v>
+      </c>
+      <c r="F99" s="10">
+        <v>608</v>
+      </c>
+      <c r="G99">
+        <v>1.5730726063406699</v>
+      </c>
+      <c r="H99">
+        <v>1.5027877315520299</v>
+      </c>
+      <c r="I99">
+        <v>1.7226080079544901</v>
+      </c>
+      <c r="J99">
+        <v>1.50996921212512</v>
+      </c>
+      <c r="K99">
+        <v>1.41805940429045</v>
+      </c>
+      <c r="L99">
+        <v>1.40442909324347</v>
+      </c>
+      <c r="M99">
+        <v>1.37950936628027</v>
+      </c>
+      <c r="N99">
+        <v>1.3396215403421601</v>
+      </c>
+      <c r="O99">
+        <v>1.2789193036500399</v>
+      </c>
+      <c r="P99">
+        <v>1.33986511878429</v>
+      </c>
+      <c r="Q99">
+        <v>1.2578451407483999</v>
+      </c>
+      <c r="R99">
+        <v>1.22652248204498</v>
+      </c>
+      <c r="S99">
+        <v>1.2637330351099401</v>
+      </c>
+      <c r="T99">
+        <v>1.39251498005039</v>
+      </c>
+      <c r="U99">
+        <v>1.2016327919200001</v>
+      </c>
+      <c r="V99">
+        <v>1.17019863840835</v>
+      </c>
+      <c r="W99">
+        <v>1.37610026033348</v>
+      </c>
+      <c r="X99">
+        <v>1.24909124509865</v>
+      </c>
+      <c r="Y99">
+        <v>1.2230539349245599</v>
+      </c>
+      <c r="Z99">
+        <v>1.6858291026024601</v>
+      </c>
+      <c r="AA99">
+        <v>1.55547438004188</v>
+      </c>
+      <c r="AB99">
+        <v>0.57128214238219099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A100" s="9">
+        <v>10</v>
+      </c>
+      <c r="B100" s="15">
+        <v>73</v>
+      </c>
+      <c r="C100" s="22">
+        <v>29</v>
+      </c>
+      <c r="D100" s="22">
+        <v>96</v>
+      </c>
+      <c r="E100" s="1">
+        <v>9</v>
+      </c>
+      <c r="F100" s="10">
+        <v>609</v>
+      </c>
+      <c r="G100">
+        <v>1.55341390227714</v>
+      </c>
+      <c r="H100">
+        <v>1.5244039225622501</v>
+      </c>
+      <c r="I100">
+        <v>1.57088108024462</v>
+      </c>
+      <c r="J100">
+        <v>1.46781066019505</v>
+      </c>
+      <c r="K100">
+        <v>1.4772812454637201</v>
+      </c>
+      <c r="L100">
+        <v>1.4628530730195799</v>
+      </c>
+      <c r="M100">
+        <v>1.4268483608354701</v>
+      </c>
+      <c r="N100">
+        <v>1.36171071518682</v>
+      </c>
+      <c r="O100">
+        <v>1.34852061203799</v>
+      </c>
+      <c r="P100">
+        <v>1.39957436101188</v>
+      </c>
+      <c r="Q100">
+        <v>1.32051490749086</v>
+      </c>
+      <c r="R100">
+        <v>1.33173415965954</v>
+      </c>
+      <c r="S100">
+        <v>1.2941330092416199</v>
+      </c>
+      <c r="T100">
+        <v>1.3355878693991401</v>
+      </c>
+      <c r="U100">
+        <v>1.26806495092404</v>
+      </c>
+      <c r="V100">
+        <v>1.2534472044821801</v>
+      </c>
+      <c r="W100">
+        <v>1.4714280564156299</v>
+      </c>
+      <c r="X100">
+        <v>1.3337840725350301</v>
+      </c>
+      <c r="Y100">
+        <v>1.28339636587065</v>
+      </c>
+      <c r="Z100">
+        <v>1.61957256436678</v>
+      </c>
+      <c r="AA100">
+        <v>1.5385431773695899</v>
+      </c>
+      <c r="AB100">
+        <v>0.51761201254014699</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
+        <v>10</v>
+      </c>
+      <c r="B101" s="15">
+        <v>65</v>
+      </c>
+      <c r="C101" s="22">
+        <v>29</v>
+      </c>
+      <c r="D101" s="22">
+        <v>96</v>
+      </c>
+      <c r="E101" s="1">
+        <v>10</v>
+      </c>
+      <c r="F101" s="10">
+        <v>610</v>
+      </c>
+      <c r="G101">
+        <v>1.3863360587251501</v>
+      </c>
+      <c r="H101">
+        <v>1.43499380870591</v>
+      </c>
+      <c r="I101">
+        <v>1.75132224817488</v>
+      </c>
+      <c r="J101">
+        <v>1.38481044361746</v>
+      </c>
+      <c r="K101">
+        <v>1.3740557222232399</v>
+      </c>
+      <c r="L101">
+        <v>1.39602945955721</v>
+      </c>
+      <c r="M101">
+        <v>1.4512619833259099</v>
+      </c>
+      <c r="N101">
+        <v>1.3466867682614001</v>
+      </c>
+      <c r="O101">
+        <v>1.37734949526511</v>
+      </c>
+      <c r="P101">
+        <v>1.2476893522977499</v>
+      </c>
+      <c r="Q101">
+        <v>1.4158739689248201</v>
+      </c>
+      <c r="R101">
+        <v>1.43277521476467</v>
+      </c>
+      <c r="S101">
+        <v>1.3874085781188501</v>
+      </c>
+      <c r="T101">
+        <v>1.3481573950427099</v>
+      </c>
+      <c r="U101">
+        <v>1.3661773137550799</v>
+      </c>
+      <c r="V101">
+        <v>1.34483469105606</v>
+      </c>
+      <c r="W101">
+        <v>1.3789189478450801</v>
+      </c>
+      <c r="X101">
+        <v>1.3618327366208201</v>
+      </c>
+      <c r="Y101">
+        <v>1.3703278654153701</v>
+      </c>
+      <c r="Z101">
+        <v>1.42436667861694</v>
+      </c>
+      <c r="AA101">
+        <v>1.3607128754963</v>
+      </c>
+      <c r="AB101">
+        <v>0.55737449591400001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>